<commit_message>
tweaks to factor analysis
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NeehaarGandhi/Desktop/STAT-363/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8768CFD1-BF89-7A4F-A74B-10BCDDBD44E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB966320-458A-2B44-BB8F-AD01C9E55B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{8E5E1190-3151-7143-9051-AD789A0B8279}"/>
   </bookViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17E1B8-668B-1540-94DD-EA54DE0B9DD1}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection sqref="A1:B49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1028,18 +1028,23 @@
       </c>
     </row>
     <row r="50" spans="1:2">
+      <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
     <row r="51" spans="1:2">
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
     <row r="52" spans="1:2">
+      <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
     <row r="53" spans="1:2">
+      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:2">
+      <c r="A54" s="1"/>
       <c r="B54" s="1"/>
     </row>
   </sheetData>

</xml_diff>